<commit_message>
Removed Files Which used for Testing
</commit_message>
<xml_diff>
--- a/data_impute_project/combinations/bird/combination_1_ABCD.xlsx
+++ b/data_impute_project/combinations/bird/combination_1_ABCD.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D178"/>
+  <dimension ref="A1:E178"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,2500 +436,3390 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>A</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>C</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>D</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>S 107</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
         <v>-19.73</v>
       </c>
-      <c r="B2" t="n">
+      <c r="C2" t="n">
         <v>10.7</v>
       </c>
-      <c r="C2" t="n">
+      <c r="D2" t="n">
         <v>-13.71</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>-6.53</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>S 108</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
         <v>-19.23</v>
       </c>
-      <c r="B3" t="n">
+      <c r="C3" t="n">
         <v>11.76</v>
       </c>
-      <c r="C3" t="n">
+      <c r="D3" t="n">
         <v>-8.390000000000001</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>-5.29</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>S 109</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
         <v>-20.87</v>
       </c>
-      <c r="B4" t="n">
+      <c r="C4" t="n">
         <v>9.57</v>
       </c>
-      <c r="C4" t="n">
+      <c r="D4" t="n">
         <v>-6.5</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>-12.15</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Hb 140</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
         <v>-20.71</v>
       </c>
-      <c r="B5" t="n">
+      <c r="C5" t="n">
         <v>8.91</v>
       </c>
-      <c r="C5" t="n">
+      <c r="D5" t="n">
         <v>-15.43</v>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
         <v>-12.74</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>S 51</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
         <v>-25.42</v>
       </c>
-      <c r="B6" t="n">
+      <c r="C6" t="n">
         <v>6.01</v>
       </c>
-      <c r="C6" t="n">
+      <c r="D6" t="n">
         <v>-14.53</v>
       </c>
-      <c r="D6" t="n">
+      <c r="E6" t="n">
         <v>-16.37</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>S 52</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
         <v>-14.78</v>
       </c>
-      <c r="B7" t="n">
+      <c r="C7" t="n">
         <v>9.56</v>
       </c>
-      <c r="C7" t="n">
+      <c r="D7" t="n">
         <v>-7.88</v>
       </c>
-      <c r="D7" t="n">
+      <c r="E7" t="n">
         <v>-7.38</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>S 54</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
         <v>-21.25</v>
       </c>
-      <c r="B8" t="n">
+      <c r="C8" t="n">
         <v>7.98</v>
       </c>
-      <c r="C8" t="n">
+      <c r="D8" t="n">
         <v>-12.07</v>
       </c>
-      <c r="D8" t="n">
+      <c r="E8" t="n">
         <v>-8.91</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>S 97</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
         <v>-21.05</v>
       </c>
-      <c r="B9" t="n">
+      <c r="C9" t="n">
         <v>4.63</v>
       </c>
-      <c r="C9" t="n">
+      <c r="D9" t="n">
         <v>-12.27</v>
       </c>
-      <c r="D9" t="n">
+      <c r="E9" t="n">
         <v>-12.38</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>113 BH1H</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
         <v>-21.19</v>
       </c>
-      <c r="B10" t="n">
+      <c r="C10" t="n">
         <v>5.76</v>
       </c>
-      <c r="C10" t="n">
+      <c r="D10" t="n">
         <v>-10.97</v>
       </c>
-      <c r="D10" t="n">
+      <c r="E10" t="n">
         <v>-5.67</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>114 BH2H</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
         <v>-20.75</v>
       </c>
-      <c r="B11" t="n">
+      <c r="C11" t="n">
         <v>6.34</v>
       </c>
-      <c r="C11" t="n">
+      <c r="D11" t="n">
         <v>-11.47</v>
       </c>
-      <c r="D11" t="n">
+      <c r="E11" t="n">
         <v>-5.89</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>117 BH5Cc</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
         <v>-21.24</v>
       </c>
-      <c r="B12" t="n">
+      <c r="C12" t="n">
         <v>4.46</v>
       </c>
-      <c r="C12" t="n">
+      <c r="D12" t="n">
         <v>-11.86</v>
       </c>
-      <c r="D12" t="n">
+      <c r="E12" t="n">
         <v>-6.73</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="n">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Hb 151</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
         <v>-22.56</v>
       </c>
-      <c r="B13" t="n">
+      <c r="C13" t="n">
         <v>8.94</v>
       </c>
-      <c r="C13" t="n">
+      <c r="D13" t="n">
         <v>-13.41</v>
       </c>
-      <c r="D13" t="n">
+      <c r="E13" t="n">
         <v>-6.8</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="n">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Hb 152</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
         <v>-21</v>
       </c>
-      <c r="B14" t="n">
+      <c r="C14" t="n">
         <v>5.54</v>
       </c>
-      <c r="C14" t="n">
+      <c r="D14" t="n">
         <v>-12.64</v>
       </c>
-      <c r="D14" t="n">
+      <c r="E14" t="n">
         <v>-11.65</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="n">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Hb 148</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
         <v>-20.75</v>
       </c>
-      <c r="B15" t="n">
+      <c r="C15" t="n">
         <v>11.68</v>
       </c>
-      <c r="C15" t="n">
+      <c r="D15" t="n">
         <v>-13.1</v>
       </c>
-      <c r="D15" t="n">
+      <c r="E15" t="n">
         <v>-11.95</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="n">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Hb 149</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
         <v>-17.01</v>
       </c>
-      <c r="B16" t="n">
+      <c r="C16" t="n">
         <v>7.61</v>
       </c>
-      <c r="C16" t="n">
+      <c r="D16" t="n">
         <v>-9.31</v>
       </c>
-      <c r="D16" t="n">
+      <c r="E16" t="n">
         <v>-13.62</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="n">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Hb 150</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
         <v>-19.21</v>
       </c>
-      <c r="B17" t="n">
+      <c r="C17" t="n">
         <v>11.13</v>
       </c>
-      <c r="C17" t="n">
+      <c r="D17" t="n">
         <v>-13.16</v>
       </c>
-      <c r="D17" t="n">
+      <c r="E17" t="n">
         <v>-6.36</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="n">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Hb 146</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
         <v>-16.57</v>
       </c>
-      <c r="B18" t="n">
+      <c r="C18" t="n">
         <v>8.140000000000001</v>
       </c>
-      <c r="C18" t="n">
+      <c r="D18" t="n">
         <v>-12.48</v>
       </c>
-      <c r="D18" t="n">
+      <c r="E18" t="n">
         <v>-12.01</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="n">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Hb 147</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
         <v>-17.1</v>
       </c>
-      <c r="B19" t="n">
+      <c r="C19" t="n">
         <v>8.619999999999999</v>
       </c>
-      <c r="C19" t="n">
+      <c r="D19" t="n">
         <v>-11.23</v>
       </c>
-      <c r="D19" t="n">
+      <c r="E19" t="n">
         <v>-9.140000000000001</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="n">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>79 EE3Tt</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
         <v>-17.08</v>
       </c>
-      <c r="B20" t="n">
+      <c r="C20" t="n">
         <v>9.029999999999999</v>
       </c>
-      <c r="C20" t="n">
+      <c r="D20" t="n">
         <v>-6.64</v>
       </c>
-      <c r="D20" t="n">
+      <c r="E20" t="n">
         <v>-8.380000000000001</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="n">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>S 76</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
         <v>-25.5</v>
       </c>
-      <c r="B21" t="n">
+      <c r="C21" t="n">
         <v>9.51</v>
       </c>
-      <c r="C21" t="n">
+      <c r="D21" t="n">
         <v>-12.86</v>
       </c>
-      <c r="D21" t="n">
+      <c r="E21" t="n">
         <v>-8.949999999999999</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="n">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>S 77</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
         <v>-12.67</v>
       </c>
-      <c r="B22" t="n">
+      <c r="C22" t="n">
         <v>13.03</v>
       </c>
-      <c r="C22" t="n">
+      <c r="D22" t="n">
         <v>-7.32</v>
       </c>
-      <c r="D22" t="n">
+      <c r="E22" t="n">
         <v>-7.68</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="n">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>S 78</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
         <v>-13.49</v>
       </c>
-      <c r="B23" t="n">
+      <c r="C23" t="n">
         <v>13.5</v>
       </c>
-      <c r="C23" t="n">
+      <c r="D23" t="n">
         <v>-6.37</v>
       </c>
-      <c r="D23" t="n">
+      <c r="E23" t="n">
         <v>-9.01</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="n">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>S 79</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
         <v>-20.75</v>
       </c>
-      <c r="B24" t="n">
+      <c r="C24" t="n">
         <v>12.05</v>
       </c>
-      <c r="C24" t="n">
+      <c r="D24" t="n">
         <v>-11.64</v>
       </c>
-      <c r="D24" t="n">
+      <c r="E24" t="n">
         <v>-6.79</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="n">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>S 80</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
         <v>-20.2</v>
       </c>
-      <c r="B25" t="n">
+      <c r="C25" t="n">
         <v>7.05</v>
       </c>
-      <c r="C25" t="n">
+      <c r="D25" t="n">
         <v>-10.65</v>
       </c>
-      <c r="D25" t="n">
+      <c r="E25" t="n">
         <v>-10.35</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="n">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>120 GS3Tt</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
         <v>-17.09</v>
       </c>
-      <c r="B26" t="n">
+      <c r="C26" t="n">
         <v>15.21</v>
       </c>
-      <c r="C26" t="n">
+      <c r="D26" t="n">
         <v>-9.140000000000001</v>
       </c>
-      <c r="D26" t="n">
+      <c r="E26" t="n">
         <v>-8.220000000000001</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="n">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>121 GS4U</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
         <v>-14.98</v>
       </c>
-      <c r="B27" t="n">
+      <c r="C27" t="n">
         <v>13.9</v>
       </c>
-      <c r="C27" t="n">
+      <c r="D27" t="n">
         <v>-8.58</v>
       </c>
-      <c r="D27" t="n">
+      <c r="E27" t="n">
         <v>-8.01</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="n">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Hb 167</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
         <v>-21.89</v>
       </c>
-      <c r="B28" t="n">
+      <c r="C28" t="n">
         <v>8.859999999999999</v>
       </c>
-      <c r="C28" t="n">
+      <c r="D28" t="n">
         <v>-15.19</v>
       </c>
-      <c r="D28" t="n">
+      <c r="E28" t="n">
         <v>-7.91</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="n">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Hb 171</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
         <v>-19.95</v>
       </c>
-      <c r="B29" t="n">
+      <c r="C29" t="n">
         <v>8.67</v>
       </c>
-      <c r="C29" t="n">
+      <c r="D29" t="n">
         <v>-13.9</v>
       </c>
-      <c r="D29" t="n">
+      <c r="E29" t="n">
         <v>-7.5</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="n">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>S 86</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
         <v>-19.23</v>
       </c>
-      <c r="B30" t="n">
+      <c r="C30" t="n">
         <v>11.86</v>
       </c>
-      <c r="C30" t="n">
+      <c r="D30" t="n">
         <v>-7.87</v>
       </c>
-      <c r="D30" t="n">
+      <c r="E30" t="n">
         <v>-6.41</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="n">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>S 87</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
         <v>-20.07</v>
       </c>
-      <c r="B31" t="n">
+      <c r="C31" t="n">
         <v>10.08</v>
       </c>
-      <c r="C31" t="n">
+      <c r="D31" t="n">
         <v>-3.17</v>
       </c>
-      <c r="D31" t="n">
+      <c r="E31" t="n">
         <v>-4.5</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="n">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>S 88</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
         <v>-20.6</v>
       </c>
-      <c r="B32" t="n">
+      <c r="C32" t="n">
         <v>8.279999999999999</v>
       </c>
-      <c r="C32" t="n">
+      <c r="D32" t="n">
         <v>-11.02</v>
       </c>
-      <c r="D32" t="n">
+      <c r="E32" t="n">
         <v>-4.83</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="n">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>S 89</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
         <v>-20.38</v>
       </c>
-      <c r="B33" t="n">
+      <c r="C33" t="n">
         <v>6.52</v>
       </c>
-      <c r="C33" t="n">
+      <c r="D33" t="n">
         <v>-9.529999999999999</v>
       </c>
-      <c r="D33" t="n">
+      <c r="E33" t="n">
         <v>-6.82</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="n">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>S 90</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
         <v>-19.16</v>
       </c>
-      <c r="B34" t="n">
+      <c r="C34" t="n">
         <v>9.26</v>
       </c>
-      <c r="C34" t="n">
+      <c r="D34" t="n">
         <v>-7.74</v>
       </c>
-      <c r="D34" t="n">
+      <c r="E34" t="n">
         <v>-6.2</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="n">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>122 HB1F</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
         <v>-20.78</v>
       </c>
-      <c r="B35" t="n">
+      <c r="C35" t="n">
         <v>11.29</v>
       </c>
-      <c r="C35" t="n">
+      <c r="D35" t="n">
         <v>-14.18</v>
       </c>
-      <c r="D35" t="n">
+      <c r="E35" t="n">
         <v>-8.24</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="n">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>123 HB2F</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
         <v>-19.91</v>
       </c>
-      <c r="B36" t="n">
+      <c r="C36" t="n">
         <v>9.18</v>
       </c>
-      <c r="C36" t="n">
+      <c r="D36" t="n">
         <v>-11.4</v>
       </c>
-      <c r="D36" t="n">
+      <c r="E36" t="n">
         <v>-6.43</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="n">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>124 HB3F</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
         <v>-20.27</v>
       </c>
-      <c r="B37" t="n">
+      <c r="C37" t="n">
         <v>6.6</v>
       </c>
-      <c r="C37" t="n">
+      <c r="D37" t="n">
         <v>-13.26</v>
       </c>
-      <c r="D37" t="n">
+      <c r="E37" t="n">
         <v>-7.27</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="n">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>125 HB4F</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
         <v>-19.08</v>
       </c>
-      <c r="B38" t="n">
+      <c r="C38" t="n">
         <v>8.58</v>
       </c>
-      <c r="C38" t="n">
+      <c r="D38" t="n">
         <v>-12.48</v>
       </c>
-      <c r="D38" t="n">
+      <c r="E38" t="n">
         <v>-4.94</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="n">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>126 HB5F</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
         <v>-19.98</v>
       </c>
-      <c r="B39" t="n">
+      <c r="C39" t="n">
         <v>10.18</v>
       </c>
-      <c r="C39" t="n">
+      <c r="D39" t="n">
         <v>-11.58</v>
       </c>
-      <c r="D39" t="n">
+      <c r="E39" t="n">
         <v>-6.87</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="n">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Hb 108</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
         <v>-21.92</v>
       </c>
-      <c r="B40" t="n">
+      <c r="C40" t="n">
         <v>8.039999999999999</v>
       </c>
-      <c r="C40" t="n">
+      <c r="D40" t="n">
         <v>-13.88</v>
       </c>
-      <c r="D40" t="n">
+      <c r="E40" t="n">
         <v>-8.119999999999999</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="n">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Hb 109</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
         <v>-22.24</v>
       </c>
-      <c r="B41" t="n">
+      <c r="C41" t="n">
         <v>7.88</v>
       </c>
-      <c r="C41" t="n">
+      <c r="D41" t="n">
         <v>-13.83</v>
       </c>
-      <c r="D41" t="n">
+      <c r="E41" t="n">
         <v>-6.81</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="n">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Hb 110</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
         <v>-23.06</v>
       </c>
-      <c r="B42" t="n">
+      <c r="C42" t="n">
         <v>7.54</v>
       </c>
-      <c r="C42" t="n">
+      <c r="D42" t="n">
         <v>-15.85</v>
       </c>
-      <c r="D42" t="n">
+      <c r="E42" t="n">
         <v>-10.36</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="n">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Hb 111</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
         <v>-23.07</v>
       </c>
-      <c r="B43" t="n">
+      <c r="C43" t="n">
         <v>10.28</v>
       </c>
-      <c r="C43" t="n">
+      <c r="D43" t="n">
         <v>-14.43</v>
       </c>
-      <c r="D43" t="n">
+      <c r="E43" t="n">
         <v>-6.04</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="n">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Hb 112</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
         <v>-21.93</v>
       </c>
-      <c r="B44" t="n">
+      <c r="C44" t="n">
         <v>6.83</v>
       </c>
-      <c r="C44" t="n">
+      <c r="D44" t="n">
         <v>-11.77</v>
       </c>
-      <c r="D44" t="n">
+      <c r="E44" t="n">
         <v>-7.02</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="n">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>S 31</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
         <v>-22.05</v>
       </c>
-      <c r="B45" t="n">
+      <c r="C45" t="n">
         <v>6.51</v>
       </c>
-      <c r="C45" t="n">
+      <c r="D45" t="n">
         <v>-13.76</v>
       </c>
-      <c r="D45" t="n">
+      <c r="E45" t="n">
         <v>-8.300000000000001</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="n">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>S 32</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
         <v>-22.58</v>
       </c>
-      <c r="B46" t="n">
+      <c r="C46" t="n">
         <v>9.4</v>
       </c>
-      <c r="C46" t="n">
+      <c r="D46" t="n">
         <v>-13.95</v>
       </c>
-      <c r="D46" t="n">
+      <c r="E46" t="n">
         <v>-7.02</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="n">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>S 33</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
         <v>-23.2</v>
       </c>
-      <c r="B47" t="n">
+      <c r="C47" t="n">
         <v>9.109999999999999</v>
       </c>
-      <c r="C47" t="n">
+      <c r="D47" t="n">
         <v>-13.83</v>
       </c>
-      <c r="D47" t="n">
+      <c r="E47" t="n">
         <v>-6.55</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="n">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>S 34</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
         <v>-21.95</v>
       </c>
-      <c r="B48" t="n">
+      <c r="C48" t="n">
         <v>7.2</v>
       </c>
-      <c r="C48" t="n">
+      <c r="D48" t="n">
         <v>-14.11</v>
       </c>
-      <c r="D48" t="n">
+      <c r="E48" t="n">
         <v>-7.68</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="n">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>S 35</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
         <v>-22.79</v>
       </c>
-      <c r="B49" t="n">
+      <c r="C49" t="n">
         <v>9.99</v>
       </c>
-      <c r="C49" t="n">
+      <c r="D49" t="n">
         <v>-14.47</v>
       </c>
-      <c r="D49" t="n">
+      <c r="E49" t="n">
         <v>-6.84</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="n">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Hb 113</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
         <v>-20.54</v>
       </c>
-      <c r="B50" t="n">
+      <c r="C50" t="n">
         <v>10.08</v>
       </c>
-      <c r="C50" t="n">
+      <c r="D50" t="n">
         <v>-12.91</v>
       </c>
-      <c r="D50" t="n">
+      <c r="E50" t="n">
         <v>-8.130000000000001</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="n">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Hb 114</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
         <v>-20.41</v>
       </c>
-      <c r="B51" t="n">
+      <c r="C51" t="n">
         <v>7.84</v>
       </c>
-      <c r="C51" t="n">
+      <c r="D51" t="n">
         <v>-14.51</v>
       </c>
-      <c r="D51" t="n">
+      <c r="E51" t="n">
         <v>-7.47</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" t="n">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Hb 115</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
         <v>-20.21</v>
       </c>
-      <c r="B52" t="n">
+      <c r="C52" t="n">
         <v>11.04</v>
       </c>
-      <c r="C52" t="n">
+      <c r="D52" t="n">
         <v>-14.27</v>
       </c>
-      <c r="D52" t="n">
+      <c r="E52" t="n">
         <v>-7.92</v>
       </c>
     </row>
     <row r="53">
-      <c r="A53" t="n">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Hb 117</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
         <v>-21.49</v>
       </c>
-      <c r="B53" t="n">
+      <c r="C53" t="n">
         <v>8.01</v>
       </c>
-      <c r="C53" t="n">
+      <c r="D53" t="n">
         <v>-13.34</v>
       </c>
-      <c r="D53" t="n">
+      <c r="E53" t="n">
         <v>-6.97</v>
       </c>
     </row>
     <row r="54">
-      <c r="A54" t="n">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>S 36</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
         <v>-20.84</v>
       </c>
-      <c r="B54" t="n">
+      <c r="C54" t="n">
         <v>7.12</v>
       </c>
-      <c r="C54" t="n">
+      <c r="D54" t="n">
         <v>-14.38</v>
       </c>
-      <c r="D54" t="n">
+      <c r="E54" t="n">
         <v>-11.22</v>
       </c>
     </row>
     <row r="55">
-      <c r="A55" t="n">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>S 37</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
         <v>-20.99</v>
       </c>
-      <c r="B55" t="n">
+      <c r="C55" t="n">
         <v>8.56</v>
       </c>
-      <c r="C55" t="n">
+      <c r="D55" t="n">
         <v>-11.82</v>
       </c>
-      <c r="D55" t="n">
+      <c r="E55" t="n">
         <v>-9.289999999999999</v>
       </c>
     </row>
     <row r="56">
-      <c r="A56" t="n">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>S 38</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
         <v>-20.46</v>
       </c>
-      <c r="B56" t="n">
+      <c r="C56" t="n">
         <v>9.15</v>
       </c>
-      <c r="C56" t="n">
+      <c r="D56" t="n">
         <v>-12.45</v>
       </c>
-      <c r="D56" t="n">
+      <c r="E56" t="n">
         <v>-6.58</v>
       </c>
     </row>
     <row r="57">
-      <c r="A57" t="n">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>S 39</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
         <v>-21.67</v>
       </c>
-      <c r="B57" t="n">
+      <c r="C57" t="n">
         <v>9.119999999999999</v>
       </c>
-      <c r="C57" t="n">
+      <c r="D57" t="n">
         <v>-13.22</v>
       </c>
-      <c r="D57" t="n">
+      <c r="E57" t="n">
         <v>-10.18</v>
       </c>
     </row>
     <row r="58">
-      <c r="A58" t="n">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>S 40</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
         <v>-21.15</v>
       </c>
-      <c r="B58" t="n">
+      <c r="C58" t="n">
         <v>7.12</v>
       </c>
-      <c r="C58" t="n">
+      <c r="D58" t="n">
         <v>-11.07</v>
       </c>
-      <c r="D58" t="n">
+      <c r="E58" t="n">
         <v>-7.15</v>
       </c>
     </row>
     <row r="59">
-      <c r="A59" t="n">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Hb 159</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
         <v>-11.41</v>
       </c>
-      <c r="B59" t="n">
+      <c r="C59" t="n">
         <v>4.6</v>
       </c>
-      <c r="C59" t="n">
+      <c r="D59" t="n">
         <v>-3.68</v>
       </c>
-      <c r="D59" t="n">
+      <c r="E59" t="n">
         <v>-6.48</v>
       </c>
     </row>
     <row r="60">
-      <c r="A60" t="n">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Hb 160</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
         <v>-20.86</v>
       </c>
-      <c r="B60" t="n">
+      <c r="C60" t="n">
         <v>12.13</v>
       </c>
-      <c r="C60" t="n">
+      <c r="D60" t="n">
         <v>-1.16</v>
       </c>
-      <c r="D60" t="n">
+      <c r="E60" t="n">
         <v>-7.13</v>
       </c>
     </row>
     <row r="61">
-      <c r="A61" t="n">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Hb 161</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
         <v>-10.61</v>
       </c>
-      <c r="B61" t="n">
+      <c r="C61" t="n">
         <v>5.13</v>
       </c>
-      <c r="C61" t="n">
+      <c r="D61" t="n">
         <v>-4.3</v>
       </c>
-      <c r="D61" t="n">
+      <c r="E61" t="n">
         <v>-10.33</v>
       </c>
     </row>
     <row r="62">
-      <c r="A62" t="n">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>80 KRA1H</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
         <v>-16.12</v>
       </c>
-      <c r="B62" t="n">
+      <c r="C62" t="n">
         <v>13.72</v>
       </c>
-      <c r="C62" t="n">
+      <c r="D62" t="n">
         <v>-5.32</v>
       </c>
-      <c r="D62" t="n">
+      <c r="E62" t="n">
         <v>-6.51</v>
       </c>
     </row>
     <row r="63">
-      <c r="A63" t="n">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>81 KRA2H</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
         <v>-21.67</v>
       </c>
-      <c r="B63" t="n">
+      <c r="C63" t="n">
         <v>10.56</v>
       </c>
-      <c r="C63" t="n">
+      <c r="D63" t="n">
         <v>-11.42</v>
       </c>
-      <c r="D63" t="n">
+      <c r="E63" t="n">
         <v>-5.62</v>
       </c>
     </row>
     <row r="64">
-      <c r="A64" t="n">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>82 KRA3H</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
         <v>-20.83</v>
       </c>
-      <c r="B64" t="n">
+      <c r="C64" t="n">
         <v>9.74</v>
       </c>
-      <c r="C64" t="n">
+      <c r="D64" t="n">
         <v>-10.38</v>
       </c>
-      <c r="D64" t="n">
+      <c r="E64" t="n">
         <v>-6.21</v>
       </c>
     </row>
     <row r="65">
-      <c r="A65" t="n">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>83 KRA4H</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
         <v>-20.67</v>
       </c>
-      <c r="B65" t="n">
+      <c r="C65" t="n">
         <v>10.94</v>
       </c>
-      <c r="C65" t="n">
+      <c r="D65" t="n">
         <v>-12.37</v>
       </c>
-      <c r="D65" t="n">
+      <c r="E65" t="n">
         <v>-6.16</v>
       </c>
     </row>
     <row r="66">
-      <c r="A66" t="n">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Hb 183</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
         <v>-20.2</v>
       </c>
-      <c r="B66" t="n">
+      <c r="C66" t="n">
         <v>11.28</v>
       </c>
-      <c r="C66" t="n">
+      <c r="D66" t="n">
         <v>-13.26</v>
       </c>
-      <c r="D66" t="n">
+      <c r="E66" t="n">
         <v>-11.15</v>
       </c>
     </row>
     <row r="67">
-      <c r="A67" t="n">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Hb 184</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
         <v>-21.07</v>
       </c>
-      <c r="B67" t="n">
+      <c r="C67" t="n">
         <v>10.54</v>
       </c>
-      <c r="C67" t="n">
+      <c r="D67" t="n">
         <v>-12.3</v>
       </c>
-      <c r="D67" t="n">
+      <c r="E67" t="n">
         <v>-6.65</v>
       </c>
     </row>
     <row r="68">
-      <c r="A68" t="n">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Hb 185</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
         <v>-19.66</v>
       </c>
-      <c r="B68" t="n">
+      <c r="C68" t="n">
         <v>12.73</v>
       </c>
-      <c r="C68" t="n">
+      <c r="D68" t="n">
         <v>-12.45</v>
       </c>
-      <c r="D68" t="n">
+      <c r="E68" t="n">
         <v>-11.54</v>
       </c>
     </row>
     <row r="69">
-      <c r="A69" t="n">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Hb 118</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
         <v>-17.45</v>
       </c>
-      <c r="B69" t="n">
+      <c r="C69" t="n">
         <v>10.38</v>
       </c>
-      <c r="C69" t="n">
+      <c r="D69" t="n">
         <v>-10.62</v>
       </c>
-      <c r="D69" t="n">
+      <c r="E69" t="n">
         <v>-7.76</v>
       </c>
     </row>
     <row r="70">
-      <c r="A70" t="n">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Hb 119</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
         <v>-13.21</v>
       </c>
-      <c r="B70" t="n">
+      <c r="C70" t="n">
         <v>11.44</v>
       </c>
-      <c r="C70" t="n">
+      <c r="D70" t="n">
         <v>-8.76</v>
       </c>
-      <c r="D70" t="n">
+      <c r="E70" t="n">
         <v>-5.25</v>
       </c>
     </row>
     <row r="71">
-      <c r="A71" t="n">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Hb 120</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
         <v>-10.25</v>
       </c>
-      <c r="B71" t="n">
+      <c r="C71" t="n">
         <v>11.98</v>
       </c>
-      <c r="C71" t="n">
+      <c r="D71" t="n">
         <v>-3.43</v>
       </c>
-      <c r="D71" t="n">
+      <c r="E71" t="n">
         <v>-11.38</v>
       </c>
     </row>
     <row r="72">
-      <c r="A72" t="n">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Hb 121</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
         <v>-12.85</v>
       </c>
-      <c r="B72" t="n">
+      <c r="C72" t="n">
         <v>11.83</v>
       </c>
-      <c r="C72" t="n">
+      <c r="D72" t="n">
         <v>-7.87</v>
       </c>
-      <c r="D72" t="n">
+      <c r="E72" t="n">
         <v>-7.37</v>
       </c>
     </row>
     <row r="73">
-      <c r="A73" t="n">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Hb 122</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
         <v>-12.54</v>
       </c>
-      <c r="B73" t="n">
+      <c r="C73" t="n">
         <v>11.38</v>
       </c>
-      <c r="C73" t="n">
+      <c r="D73" t="n">
         <v>-8.25</v>
       </c>
-      <c r="D73" t="n">
+      <c r="E73" t="n">
         <v>-8.15</v>
       </c>
     </row>
     <row r="74">
-      <c r="A74" t="n">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>86 K2H</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
         <v>-14.85</v>
       </c>
-      <c r="B74" t="n">
+      <c r="C74" t="n">
         <v>11.53</v>
       </c>
-      <c r="C74" t="n">
+      <c r="D74" t="n">
         <v>-7.37</v>
       </c>
-      <c r="D74" t="n">
+      <c r="E74" t="n">
         <v>-7.63</v>
       </c>
     </row>
     <row r="75">
-      <c r="A75" t="n">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>87 K3F</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
         <v>-14.29</v>
       </c>
-      <c r="B75" t="n">
+      <c r="C75" t="n">
         <v>12.38</v>
       </c>
-      <c r="C75" t="n">
+      <c r="D75" t="n">
         <v>-6.37</v>
       </c>
-      <c r="D75" t="n">
+      <c r="E75" t="n">
         <v>-6.51</v>
       </c>
     </row>
     <row r="76">
-      <c r="A76" t="n">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>88 K4Cc</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
         <v>-17</v>
       </c>
-      <c r="B76" t="n">
+      <c r="C76" t="n">
         <v>11.63</v>
       </c>
-      <c r="C76" t="n">
+      <c r="D76" t="n">
         <v>-8.59</v>
       </c>
-      <c r="D76" t="n">
+      <c r="E76" t="n">
         <v>-8.42</v>
       </c>
     </row>
     <row r="77">
-      <c r="A77" t="n">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>89 K5U</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
         <v>-14.34</v>
       </c>
-      <c r="B77" t="n">
+      <c r="C77" t="n">
         <v>12.18</v>
       </c>
-      <c r="C77" t="n">
+      <c r="D77" t="n">
         <v>-9.26</v>
       </c>
-      <c r="D77" t="n">
+      <c r="E77" t="n">
         <v>-6.97</v>
       </c>
     </row>
     <row r="78">
-      <c r="A78" t="n">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>S 101</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
         <v>-20.92</v>
       </c>
-      <c r="B78" t="n">
+      <c r="C78" t="n">
         <v>10.51</v>
       </c>
-      <c r="C78" t="n">
+      <c r="D78" t="n">
         <v>-10.56</v>
       </c>
-      <c r="D78" t="n">
+      <c r="E78" t="n">
         <v>-7.33</v>
       </c>
     </row>
     <row r="79">
-      <c r="A79" t="n">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>S 102</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
         <v>-25</v>
       </c>
-      <c r="B79" t="n">
+      <c r="C79" t="n">
         <v>9.449999999999999</v>
       </c>
-      <c r="C79" t="n">
+      <c r="D79" t="n">
         <v>-6.12</v>
       </c>
-      <c r="D79" t="n">
+      <c r="E79" t="n">
         <v>-11.59</v>
       </c>
     </row>
     <row r="80">
-      <c r="A80" t="n">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>127 KN1Tt</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
         <v>-20.07</v>
       </c>
-      <c r="B80" t="n">
+      <c r="C80" t="n">
         <v>9.029999999999999</v>
       </c>
-      <c r="C80" t="n">
+      <c r="D80" t="n">
         <v>-10.64</v>
       </c>
-      <c r="D80" t="n">
+      <c r="E80" t="n">
         <v>-5.21</v>
       </c>
     </row>
     <row r="81">
-      <c r="A81" t="n">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>128 KN2Tt</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
         <v>-21.22</v>
       </c>
-      <c r="B81" t="n">
+      <c r="C81" t="n">
         <v>10.06</v>
       </c>
-      <c r="C81" t="n">
+      <c r="D81" t="n">
         <v>-14.08</v>
       </c>
-      <c r="D81" t="n">
+      <c r="E81" t="n">
         <v>-5.57</v>
       </c>
     </row>
     <row r="82">
-      <c r="A82" t="n">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>129 KN3Tt</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
         <v>-24.17</v>
       </c>
-      <c r="B82" t="n">
+      <c r="C82" t="n">
         <v>10.06</v>
       </c>
-      <c r="C82" t="n">
+      <c r="D82" t="n">
         <v>-7.49</v>
       </c>
-      <c r="D82" t="n">
+      <c r="E82" t="n">
         <v>-12.5</v>
       </c>
     </row>
     <row r="83">
-      <c r="A83" t="n">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>130 KN4U</t>
+        </is>
+      </c>
+      <c r="B83" t="n">
         <v>-19.05</v>
       </c>
-      <c r="B83" t="n">
+      <c r="C83" t="n">
         <v>9.640000000000001</v>
       </c>
-      <c r="C83" t="n">
+      <c r="D83" t="n">
         <v>-11.78</v>
       </c>
-      <c r="D83" t="n">
+      <c r="E83" t="n">
         <v>-6.16</v>
       </c>
     </row>
     <row r="84">
-      <c r="A84" t="n">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>131 KN5Cr</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
         <v>-19.3</v>
       </c>
-      <c r="B84" t="n">
+      <c r="C84" t="n">
         <v>10.36</v>
       </c>
-      <c r="C84" t="n">
+      <c r="D84" t="n">
         <v>-11.09</v>
       </c>
-      <c r="D84" t="n">
+      <c r="E84" t="n">
         <v>-6.42</v>
       </c>
     </row>
     <row r="85">
-      <c r="A85" t="n">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>S 71</t>
+        </is>
+      </c>
+      <c r="B85" t="n">
         <v>-12.6</v>
       </c>
-      <c r="B85" t="n">
+      <c r="C85" t="n">
         <v>11.09</v>
       </c>
-      <c r="C85" t="n">
+      <c r="D85" t="n">
         <v>-7.78</v>
       </c>
-      <c r="D85" t="n">
+      <c r="E85" t="n">
         <v>-12.45</v>
       </c>
     </row>
     <row r="86">
-      <c r="A86" t="n">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>S 72</t>
+        </is>
+      </c>
+      <c r="B86" t="n">
         <v>-20.47</v>
       </c>
-      <c r="B86" t="n">
+      <c r="C86" t="n">
         <v>6.36</v>
       </c>
-      <c r="C86" t="n">
+      <c r="D86" t="n">
         <v>-11.17</v>
       </c>
-      <c r="D86" t="n">
+      <c r="E86" t="n">
         <v>-11.09</v>
       </c>
     </row>
     <row r="87">
-      <c r="A87" t="n">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>S 73</t>
+        </is>
+      </c>
+      <c r="B87" t="n">
         <v>-20.67</v>
       </c>
-      <c r="B87" t="n">
+      <c r="C87" t="n">
         <v>8.779999999999999</v>
       </c>
-      <c r="C87" t="n">
+      <c r="D87" t="n">
         <v>-11.92</v>
       </c>
-      <c r="D87" t="n">
+      <c r="E87" t="n">
         <v>-9.199999999999999</v>
       </c>
     </row>
     <row r="88">
-      <c r="A88" t="n">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>S 74</t>
+        </is>
+      </c>
+      <c r="B88" t="n">
         <v>-13.53</v>
       </c>
-      <c r="B88" t="n">
+      <c r="C88" t="n">
         <v>11.33</v>
       </c>
-      <c r="C88" t="n">
+      <c r="D88" t="n">
         <v>-7.58</v>
       </c>
-      <c r="D88" t="n">
+      <c r="E88" t="n">
         <v>-8.84</v>
       </c>
     </row>
     <row r="89">
-      <c r="A89" t="n">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>S 75</t>
+        </is>
+      </c>
+      <c r="B89" t="n">
         <v>-14.93</v>
       </c>
-      <c r="B89" t="n">
+      <c r="C89" t="n">
         <v>12.67</v>
       </c>
-      <c r="C89" t="n">
+      <c r="D89" t="n">
         <v>-9.109999999999999</v>
       </c>
-      <c r="D89" t="n">
+      <c r="E89" t="n">
         <v>-7.25</v>
       </c>
     </row>
     <row r="90">
-      <c r="A90" t="n">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>Hb 126</t>
+        </is>
+      </c>
+      <c r="B90" t="n">
         <v>-22.96</v>
       </c>
-      <c r="B90" t="n">
+      <c r="C90" t="n">
         <v>8.43</v>
       </c>
-      <c r="C90" t="n">
+      <c r="D90" t="n">
         <v>-15.46</v>
       </c>
-      <c r="D90" t="n">
+      <c r="E90" t="n">
         <v>-13.56</v>
       </c>
     </row>
     <row r="91">
-      <c r="A91" t="n">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>Hb 127</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
         <v>-23.03</v>
       </c>
-      <c r="B91" t="n">
+      <c r="C91" t="n">
         <v>5.22</v>
       </c>
-      <c r="C91" t="n">
+      <c r="D91" t="n">
         <v>-13.52</v>
       </c>
-      <c r="D91" t="n">
+      <c r="E91" t="n">
         <v>-11.92</v>
       </c>
     </row>
     <row r="92">
-      <c r="A92" t="n">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>Hb 136</t>
+        </is>
+      </c>
+      <c r="B92" t="n">
         <v>-25.46</v>
       </c>
-      <c r="B92" t="n">
+      <c r="C92" t="n">
         <v>9.26</v>
       </c>
-      <c r="C92" t="n">
+      <c r="D92" t="n">
         <v>-18.49</v>
       </c>
-      <c r="D92" t="n">
+      <c r="E92" t="n">
         <v>-11.49</v>
       </c>
     </row>
     <row r="93">
-      <c r="A93" t="n">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>Hb 138</t>
+        </is>
+      </c>
+      <c r="B93" t="n">
         <v>-21.03</v>
       </c>
-      <c r="B93" t="n">
+      <c r="C93" t="n">
         <v>7.49</v>
       </c>
-      <c r="C93" t="n">
+      <c r="D93" t="n">
         <v>-13.73</v>
       </c>
-      <c r="D93" t="n">
+      <c r="E93" t="n">
         <v>-10.83</v>
       </c>
     </row>
     <row r="94">
-      <c r="A94" t="n">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>Hb 139</t>
+        </is>
+      </c>
+      <c r="B94" t="n">
         <v>-21.36</v>
       </c>
-      <c r="B94" t="n">
+      <c r="C94" t="n">
         <v>8.119999999999999</v>
       </c>
-      <c r="C94" t="n">
+      <c r="D94" t="n">
         <v>-13.06</v>
       </c>
-      <c r="D94" t="n">
+      <c r="E94" t="n">
         <v>-8.609999999999999</v>
       </c>
     </row>
     <row r="95">
-      <c r="A95" t="n">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>90 RE1H</t>
+        </is>
+      </c>
+      <c r="B95" t="n">
         <v>-22.79</v>
       </c>
-      <c r="B95" t="n">
+      <c r="C95" t="n">
         <v>7.02</v>
       </c>
-      <c r="C95" t="n">
+      <c r="D95" t="n">
         <v>-12.19</v>
       </c>
-      <c r="D95" t="n">
+      <c r="E95" t="n">
         <v>-10.13</v>
       </c>
     </row>
     <row r="96">
-      <c r="A96" t="n">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>91 RE2Tt</t>
+        </is>
+      </c>
+      <c r="B96" t="n">
         <v>-10.77</v>
       </c>
-      <c r="B96" t="n">
+      <c r="C96" t="n">
         <v>7.57</v>
       </c>
-      <c r="C96" t="n">
+      <c r="D96" t="n">
         <v>-3.18</v>
       </c>
-      <c r="D96" t="n">
+      <c r="E96" t="n">
         <v>-12.97</v>
       </c>
     </row>
     <row r="97">
-      <c r="A97" t="n">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>92 RE3St</t>
+        </is>
+      </c>
+      <c r="B97" t="n">
         <v>-22.61</v>
       </c>
-      <c r="B97" t="n">
+      <c r="C97" t="n">
         <v>9.82</v>
       </c>
-      <c r="C97" t="n">
+      <c r="D97" t="n">
         <v>-10.95</v>
       </c>
-      <c r="D97" t="n">
+      <c r="E97" t="n">
         <v>-11.49</v>
       </c>
     </row>
     <row r="98">
-      <c r="A98" t="n">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>132 RE1H</t>
+        </is>
+      </c>
+      <c r="B98" t="n">
         <v>-19.31</v>
       </c>
-      <c r="B98" t="n">
+      <c r="C98" t="n">
         <v>7.34</v>
       </c>
-      <c r="C98" t="n">
+      <c r="D98" t="n">
         <v>-12.32</v>
       </c>
-      <c r="D98" t="n">
+      <c r="E98" t="n">
         <v>-10.24</v>
       </c>
     </row>
     <row r="99">
-      <c r="A99" t="n">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>133 RE2H</t>
+        </is>
+      </c>
+      <c r="B99" t="n">
         <v>-24.12</v>
       </c>
-      <c r="B99" t="n">
+      <c r="C99" t="n">
         <v>8.609999999999999</v>
       </c>
-      <c r="C99" t="n">
+      <c r="D99" t="n">
         <v>-16.81</v>
       </c>
-      <c r="D99" t="n">
+      <c r="E99" t="n">
         <v>-13.05</v>
       </c>
     </row>
     <row r="100">
-      <c r="A100" t="n">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>134 RE3H</t>
+        </is>
+      </c>
+      <c r="B100" t="n">
         <v>-25.76</v>
       </c>
-      <c r="B100" t="n">
+      <c r="C100" t="n">
         <v>7.03</v>
       </c>
-      <c r="C100" t="n">
+      <c r="D100" t="n">
         <v>-16.5</v>
       </c>
-      <c r="D100" t="n">
+      <c r="E100" t="n">
         <v>-10.84</v>
       </c>
     </row>
     <row r="101">
-      <c r="A101" t="n">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>135 RE4H</t>
+        </is>
+      </c>
+      <c r="B101" t="n">
         <v>-30.51</v>
       </c>
-      <c r="B101" t="n">
+      <c r="C101" t="n">
         <v>9.44</v>
       </c>
-      <c r="C101" t="n">
+      <c r="D101" t="n">
         <v>-19.36</v>
       </c>
-      <c r="D101" t="n">
+      <c r="E101" t="n">
         <v>-12.51</v>
       </c>
     </row>
     <row r="102">
-      <c r="A102" t="n">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>136 RE5H</t>
+        </is>
+      </c>
+      <c r="B102" t="n">
         <v>-20.29</v>
       </c>
-      <c r="B102" t="n">
+      <c r="C102" t="n">
         <v>7.71</v>
       </c>
-      <c r="C102" t="n">
+      <c r="D102" t="n">
         <v>-12.75</v>
       </c>
-      <c r="D102" t="n">
+      <c r="E102" t="n">
         <v>-8.289999999999999</v>
       </c>
     </row>
     <row r="103">
-      <c r="A103" t="n">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>Hb 142</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
         <v>-23.79</v>
       </c>
-      <c r="B103" t="n">
+      <c r="C103" t="n">
         <v>7.25</v>
       </c>
-      <c r="C103" t="n">
+      <c r="D103" t="n">
         <v>-16.13</v>
       </c>
-      <c r="D103" t="n">
+      <c r="E103" t="n">
         <v>-7.98</v>
       </c>
     </row>
     <row r="104">
-      <c r="A104" t="n">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>S 61</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
         <v>-22.34</v>
       </c>
-      <c r="B104" t="n">
+      <c r="C104" t="n">
         <v>8.539999999999999</v>
       </c>
-      <c r="C104" t="n">
+      <c r="D104" t="n">
         <v>-15.7</v>
       </c>
-      <c r="D104" t="n">
+      <c r="E104" t="n">
         <v>-7.3</v>
       </c>
     </row>
     <row r="105">
-      <c r="A105" t="n">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>S 62</t>
+        </is>
+      </c>
+      <c r="B105" t="n">
         <v>-19.06</v>
       </c>
-      <c r="B105" t="n">
+      <c r="C105" t="n">
         <v>8.109999999999999</v>
       </c>
-      <c r="C105" t="n">
+      <c r="D105" t="n">
         <v>-8.960000000000001</v>
       </c>
-      <c r="D105" t="n">
+      <c r="E105" t="n">
         <v>-7.25</v>
       </c>
     </row>
     <row r="106">
-      <c r="A106" t="n">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>S 63</t>
+        </is>
+      </c>
+      <c r="B106" t="n">
         <v>-22.69</v>
       </c>
-      <c r="B106" t="n">
+      <c r="C106" t="n">
         <v>8.49</v>
       </c>
-      <c r="C106" t="n">
+      <c r="D106" t="n">
         <v>-12.86</v>
       </c>
-      <c r="D106" t="n">
+      <c r="E106" t="n">
         <v>-7.88</v>
       </c>
     </row>
     <row r="107">
-      <c r="A107" t="n">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>S 65</t>
+        </is>
+      </c>
+      <c r="B107" t="n">
         <v>-18.91</v>
       </c>
-      <c r="B107" t="n">
+      <c r="C107" t="n">
         <v>7.63</v>
       </c>
-      <c r="C107" t="n">
+      <c r="D107" t="n">
         <v>-12.93</v>
       </c>
-      <c r="D107" t="n">
+      <c r="E107" t="n">
         <v>-10.36</v>
       </c>
     </row>
     <row r="108">
-      <c r="A108" t="n">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>137 SC1H</t>
+        </is>
+      </c>
+      <c r="B108" t="n">
         <v>-18.31</v>
       </c>
-      <c r="B108" t="n">
+      <c r="C108" t="n">
         <v>10.78</v>
       </c>
-      <c r="C108" t="n">
+      <c r="D108" t="n">
         <v>-10.75</v>
       </c>
-      <c r="D108" t="n">
+      <c r="E108" t="n">
         <v>-8.58</v>
       </c>
     </row>
     <row r="109">
-      <c r="A109" t="n">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>138 SC2H</t>
+        </is>
+      </c>
+      <c r="B109" t="n">
         <v>-21.61</v>
       </c>
-      <c r="B109" t="n">
+      <c r="C109" t="n">
         <v>7.07</v>
       </c>
-      <c r="C109" t="n">
+      <c r="D109" t="n">
         <v>-12.06</v>
       </c>
-      <c r="D109" t="n">
+      <c r="E109" t="n">
         <v>-9.19</v>
       </c>
     </row>
     <row r="110">
-      <c r="A110" t="n">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>139 SC3H</t>
+        </is>
+      </c>
+      <c r="B110" t="n">
         <v>-26.65</v>
       </c>
-      <c r="B110" t="n">
+      <c r="C110" t="n">
         <v>8.33</v>
       </c>
-      <c r="C110" t="n">
+      <c r="D110" t="n">
         <v>-16.53</v>
       </c>
-      <c r="D110" t="n">
+      <c r="E110" t="n">
         <v>-10.11</v>
       </c>
     </row>
     <row r="111">
-      <c r="A111" t="n">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>140 SC4H</t>
+        </is>
+      </c>
+      <c r="B111" t="n">
         <v>-21.96</v>
       </c>
-      <c r="B111" t="n">
+      <c r="C111" t="n">
         <v>8.109999999999999</v>
       </c>
-      <c r="C111" t="n">
+      <c r="D111" t="n">
         <v>-13.53</v>
       </c>
-      <c r="D111" t="n">
+      <c r="E111" t="n">
         <v>-11.31</v>
       </c>
     </row>
     <row r="112">
-      <c r="A112" t="n">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>141 SC5H</t>
+        </is>
+      </c>
+      <c r="B112" t="n">
         <v>-18.81</v>
       </c>
-      <c r="B112" t="n">
+      <c r="C112" t="n">
         <v>9.19</v>
       </c>
-      <c r="C112" t="n">
+      <c r="D112" t="n">
         <v>-10.18</v>
       </c>
-      <c r="D112" t="n">
+      <c r="E112" t="n">
         <v>-10.27</v>
       </c>
     </row>
     <row r="113">
-      <c r="A113" t="n">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>Hb 162</t>
+        </is>
+      </c>
+      <c r="B113" t="n">
         <v>-19.87</v>
       </c>
-      <c r="B113" t="n">
+      <c r="C113" t="n">
         <v>11.77</v>
       </c>
-      <c r="C113" t="n">
+      <c r="D113" t="n">
         <v>-23.54</v>
       </c>
-      <c r="D113" t="n">
+      <c r="E113" t="n">
         <v>-8.029999999999999</v>
       </c>
     </row>
     <row r="114">
-      <c r="A114" t="n">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>Hb 163</t>
+        </is>
+      </c>
+      <c r="B114" t="n">
         <v>-19.91</v>
       </c>
-      <c r="B114" t="n">
+      <c r="C114" t="n">
         <v>10.97</v>
       </c>
-      <c r="C114" t="n">
+      <c r="D114" t="n">
         <v>-13.73</v>
       </c>
-      <c r="D114" t="n">
+      <c r="E114" t="n">
         <v>-10.07</v>
       </c>
     </row>
     <row r="115">
-      <c r="A115" t="n">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>Hb 164</t>
+        </is>
+      </c>
+      <c r="B115" t="n">
         <v>-24.93</v>
       </c>
-      <c r="B115" t="n">
+      <c r="C115" t="n">
         <v>9.92</v>
       </c>
-      <c r="C115" t="n">
+      <c r="D115" t="n">
         <v>-13.74</v>
       </c>
-      <c r="D115" t="n">
+      <c r="E115" t="n">
         <v>-9.390000000000001</v>
       </c>
     </row>
     <row r="116">
-      <c r="A116" t="n">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>Hb 166</t>
+        </is>
+      </c>
+      <c r="B116" t="n">
         <v>-17.53</v>
       </c>
-      <c r="B116" t="n">
+      <c r="C116" t="n">
         <v>11.46</v>
       </c>
-      <c r="C116" t="n">
+      <c r="D116" t="n">
         <v>-9.56</v>
       </c>
-      <c r="D116" t="n">
+      <c r="E116" t="n">
         <v>-8.710000000000001</v>
       </c>
     </row>
     <row r="117">
-      <c r="A117" t="n">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>S 81</t>
+        </is>
+      </c>
+      <c r="B117" t="n">
         <v>-20.18</v>
       </c>
-      <c r="B117" t="n">
+      <c r="C117" t="n">
         <v>10.32</v>
       </c>
-      <c r="C117" t="n">
+      <c r="D117" t="n">
         <v>-9.68</v>
       </c>
-      <c r="D117" t="n">
+      <c r="E117" t="n">
         <v>-5.26</v>
       </c>
     </row>
     <row r="118">
-      <c r="A118" t="n">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>S 82</t>
+        </is>
+      </c>
+      <c r="B118" t="n">
         <v>-16.55</v>
       </c>
-      <c r="B118" t="n">
+      <c r="C118" t="n">
         <v>10.83</v>
       </c>
-      <c r="C118" t="n">
+      <c r="D118" t="n">
         <v>-8.74</v>
       </c>
-      <c r="D118" t="n">
+      <c r="E118" t="n">
         <v>-8.039999999999999</v>
       </c>
     </row>
     <row r="119">
-      <c r="A119" t="n">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>S 83</t>
+        </is>
+      </c>
+      <c r="B119" t="n">
         <v>-12.41</v>
       </c>
-      <c r="B119" t="n">
+      <c r="C119" t="n">
         <v>11.83</v>
       </c>
-      <c r="C119" t="n">
+      <c r="D119" t="n">
         <v>-5.03</v>
       </c>
-      <c r="D119" t="n">
+      <c r="E119" t="n">
         <v>-10.28</v>
       </c>
     </row>
     <row r="120">
-      <c r="A120" t="n">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>S 84</t>
+        </is>
+      </c>
+      <c r="B120" t="n">
         <v>-20.47</v>
       </c>
-      <c r="B120" t="n">
+      <c r="C120" t="n">
         <v>9.869999999999999</v>
       </c>
-      <c r="C120" t="n">
+      <c r="D120" t="n">
         <v>-8.890000000000001</v>
       </c>
-      <c r="D120" t="n">
+      <c r="E120" t="n">
         <v>-8.449999999999999</v>
       </c>
     </row>
     <row r="121">
-      <c r="A121" t="n">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>S 85</t>
+        </is>
+      </c>
+      <c r="B121" t="n">
         <v>-15.56</v>
       </c>
-      <c r="B121" t="n">
+      <c r="C121" t="n">
         <v>12.64</v>
       </c>
-      <c r="C121" t="n">
+      <c r="D121" t="n">
         <v>-7.06</v>
       </c>
-      <c r="D121" t="n">
+      <c r="E121" t="n">
         <v>-7.37</v>
       </c>
     </row>
     <row r="122">
-      <c r="A122" t="n">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>93 SA1U</t>
+        </is>
+      </c>
+      <c r="B122" t="n">
         <v>-19.88</v>
       </c>
-      <c r="B122" t="n">
+      <c r="C122" t="n">
         <v>1.25</v>
       </c>
-      <c r="C122" t="n">
+      <c r="D122" t="n">
         <v>-11.41</v>
       </c>
-      <c r="D122" t="n">
+      <c r="E122" t="n">
         <v>-11.65</v>
       </c>
     </row>
     <row r="123">
-      <c r="A123" t="n">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>94 SA2U</t>
+        </is>
+      </c>
+      <c r="B123" t="n">
         <v>-18.2</v>
       </c>
-      <c r="B123" t="n">
+      <c r="C123" t="n">
         <v>11.02</v>
       </c>
-      <c r="C123" t="n">
+      <c r="D123" t="n">
         <v>-9.210000000000001</v>
       </c>
-      <c r="D123" t="n">
+      <c r="E123" t="n">
         <v>-8.93</v>
       </c>
     </row>
     <row r="124">
-      <c r="A124" t="n">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>95 SA3U</t>
+        </is>
+      </c>
+      <c r="B124" t="n">
         <v>-19.54</v>
       </c>
-      <c r="B124" t="n">
+      <c r="C124" t="n">
         <v>11.41</v>
       </c>
-      <c r="C124" t="n">
+      <c r="D124" t="n">
         <v>-11.24</v>
       </c>
-      <c r="D124" t="n">
+      <c r="E124" t="n">
         <v>-9.73</v>
       </c>
     </row>
     <row r="125">
-      <c r="A125" t="n">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>96 SA4U</t>
+        </is>
+      </c>
+      <c r="B125" t="n">
         <v>-12.1</v>
       </c>
-      <c r="B125" t="n">
+      <c r="C125" t="n">
         <v>13.51</v>
       </c>
-      <c r="C125" t="n">
+      <c r="D125" t="n">
         <v>-6.2</v>
       </c>
-      <c r="D125" t="n">
+      <c r="E125" t="n">
         <v>-5.94</v>
       </c>
     </row>
     <row r="126">
-      <c r="A126" t="n">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>97 SA5H</t>
+        </is>
+      </c>
+      <c r="B126" t="n">
         <v>-16.11</v>
       </c>
-      <c r="B126" t="n">
+      <c r="C126" t="n">
         <v>13.45</v>
       </c>
-      <c r="C126" t="n">
+      <c r="D126" t="n">
         <v>-6</v>
       </c>
-      <c r="D126" t="n">
+      <c r="E126" t="n">
         <v>-5.9</v>
       </c>
     </row>
     <row r="127">
-      <c r="A127" t="n">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>142 SA1H</t>
+        </is>
+      </c>
+      <c r="B127" t="n">
         <v>-22.37</v>
       </c>
-      <c r="B127" t="n">
+      <c r="C127" t="n">
         <v>13.1</v>
       </c>
-      <c r="C127" t="n">
+      <c r="D127" t="n">
         <v>-13.92</v>
       </c>
-      <c r="D127" t="n">
+      <c r="E127" t="n">
         <v>-6.55</v>
       </c>
     </row>
     <row r="128">
-      <c r="A128" t="n">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>144 SA3Tt</t>
+        </is>
+      </c>
+      <c r="B128" t="n">
         <v>-12.45</v>
       </c>
-      <c r="B128" t="n">
+      <c r="C128" t="n">
         <v>12.83</v>
       </c>
-      <c r="C128" t="n">
+      <c r="D128" t="n">
         <v>-2.33</v>
       </c>
-      <c r="D128" t="n">
+      <c r="E128" t="n">
         <v>-6.39</v>
       </c>
     </row>
     <row r="129">
-      <c r="A129" t="n">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>146 SA5Cmc</t>
+        </is>
+      </c>
+      <c r="B129" t="n">
         <v>-13.24</v>
       </c>
-      <c r="B129" t="n">
+      <c r="C129" t="n">
         <v>12.2</v>
       </c>
-      <c r="C129" t="n">
+      <c r="D129" t="n">
         <v>-6.64</v>
       </c>
-      <c r="D129" t="n">
+      <c r="E129" t="n">
         <v>-6.12</v>
       </c>
     </row>
     <row r="130">
-      <c r="A130" t="n">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>Hb 153</t>
+        </is>
+      </c>
+      <c r="B130" t="n">
         <v>-17.69</v>
       </c>
-      <c r="B130" t="n">
+      <c r="C130" t="n">
         <v>7.95</v>
       </c>
-      <c r="C130" t="n">
+      <c r="D130" t="n">
         <v>-8.869999999999999</v>
       </c>
-      <c r="D130" t="n">
+      <c r="E130" t="n">
         <v>-9.619999999999999</v>
       </c>
     </row>
     <row r="131">
-      <c r="A131" t="n">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>Hb 154</t>
+        </is>
+      </c>
+      <c r="B131" t="n">
         <v>-21.9</v>
       </c>
-      <c r="B131" t="n">
+      <c r="C131" t="n">
         <v>8.25</v>
       </c>
-      <c r="C131" t="n">
+      <c r="D131" t="n">
         <v>-13.89</v>
       </c>
-      <c r="D131" t="n">
+      <c r="E131" t="n">
         <v>-10.15</v>
       </c>
     </row>
     <row r="132">
-      <c r="A132" t="n">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>Hb 155</t>
+        </is>
+      </c>
+      <c r="B132" t="n">
         <v>-21.6</v>
       </c>
-      <c r="B132" t="n">
+      <c r="C132" t="n">
         <v>7.33</v>
       </c>
-      <c r="C132" t="n">
+      <c r="D132" t="n">
         <v>-13.78</v>
       </c>
-      <c r="D132" t="n">
+      <c r="E132" t="n">
         <v>-9.859999999999999</v>
       </c>
     </row>
     <row r="133">
-      <c r="A133" t="n">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>Hb 156</t>
+        </is>
+      </c>
+      <c r="B133" t="n">
         <v>-19</v>
       </c>
-      <c r="B133" t="n">
+      <c r="C133" t="n">
         <v>6.36</v>
       </c>
-      <c r="C133" t="n">
+      <c r="D133" t="n">
         <v>-6.82</v>
       </c>
-      <c r="D133" t="n">
+      <c r="E133" t="n">
         <v>-9.359999999999999</v>
       </c>
     </row>
     <row r="134">
-      <c r="A134" t="n">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>S 41</t>
+        </is>
+      </c>
+      <c r="B134" t="n">
         <v>-19.68</v>
       </c>
-      <c r="B134" t="n">
+      <c r="C134" t="n">
         <v>6.42</v>
       </c>
-      <c r="C134" t="n">
+      <c r="D134" t="n">
         <v>-8.32</v>
       </c>
-      <c r="D134" t="n">
+      <c r="E134" t="n">
         <v>-9.57</v>
       </c>
     </row>
     <row r="135">
-      <c r="A135" t="n">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>S 42</t>
+        </is>
+      </c>
+      <c r="B135" t="n">
         <v>-19.39</v>
       </c>
-      <c r="B135" t="n">
+      <c r="C135" t="n">
         <v>4.29</v>
       </c>
-      <c r="C135" t="n">
+      <c r="D135" t="n">
         <v>-7.6</v>
       </c>
-      <c r="D135" t="n">
+      <c r="E135" t="n">
         <v>-12.21</v>
       </c>
     </row>
     <row r="136">
-      <c r="A136" t="n">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>S 43</t>
+        </is>
+      </c>
+      <c r="B136" t="n">
         <v>-23.62</v>
       </c>
-      <c r="B136" t="n">
+      <c r="C136" t="n">
         <v>7.97</v>
       </c>
-      <c r="C136" t="n">
+      <c r="D136" t="n">
         <v>-12.53</v>
       </c>
-      <c r="D136" t="n">
+      <c r="E136" t="n">
         <v>-11.75</v>
       </c>
     </row>
     <row r="137">
-      <c r="A137" t="n">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>S 44</t>
+        </is>
+      </c>
+      <c r="B137" t="n">
         <v>-21.55</v>
       </c>
-      <c r="B137" t="n">
+      <c r="C137" t="n">
         <v>6.64</v>
       </c>
-      <c r="C137" t="n">
+      <c r="D137" t="n">
         <v>-12.88</v>
       </c>
-      <c r="D137" t="n">
+      <c r="E137" t="n">
         <v>-11.03</v>
       </c>
     </row>
     <row r="138">
-      <c r="A138" t="n">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>S 45</t>
+        </is>
+      </c>
+      <c r="B138" t="n">
         <v>-16.01</v>
       </c>
-      <c r="B138" t="n">
+      <c r="C138" t="n">
         <v>5.71</v>
       </c>
-      <c r="C138" t="n">
+      <c r="D138" t="n">
         <v>-8.73</v>
       </c>
-      <c r="D138" t="n">
+      <c r="E138" t="n">
         <v>-11.63</v>
       </c>
     </row>
     <row r="139">
-      <c r="A139" t="n">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>98 SW1H</t>
+        </is>
+      </c>
+      <c r="B139" t="n">
         <v>-20.08</v>
       </c>
-      <c r="B139" t="n">
+      <c r="C139" t="n">
         <v>7.21</v>
       </c>
-      <c r="C139" t="n">
+      <c r="D139" t="n">
         <v>-10.58</v>
       </c>
-      <c r="D139" t="n">
+      <c r="E139" t="n">
         <v>-10.95</v>
       </c>
     </row>
     <row r="140">
-      <c r="A140" t="n">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>99 SW2Cc</t>
+        </is>
+      </c>
+      <c r="B140" t="n">
         <v>-18.32</v>
       </c>
-      <c r="B140" t="n">
+      <c r="C140" t="n">
         <v>3.78</v>
       </c>
-      <c r="C140" t="n">
+      <c r="D140" t="n">
         <v>-5.5</v>
       </c>
-      <c r="D140" t="n">
+      <c r="E140" t="n">
         <v>-7.41</v>
       </c>
     </row>
     <row r="141">
-      <c r="A141" t="n">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>100 SW3R</t>
+        </is>
+      </c>
+      <c r="B141" t="n">
         <v>-16.69</v>
       </c>
-      <c r="B141" t="n">
+      <c r="C141" t="n">
         <v>5.08</v>
       </c>
-      <c r="C141" t="n">
+      <c r="D141" t="n">
         <v>-8.44</v>
       </c>
-      <c r="D141" t="n">
+      <c r="E141" t="n">
         <v>-6.92</v>
       </c>
     </row>
     <row r="142">
-      <c r="A142" t="n">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>147 SW1R</t>
+        </is>
+      </c>
+      <c r="B142" t="n">
         <v>-20.57</v>
       </c>
-      <c r="B142" t="n">
+      <c r="C142" t="n">
         <v>7.03</v>
       </c>
-      <c r="C142" t="n">
+      <c r="D142" t="n">
         <v>-11.02</v>
       </c>
-      <c r="D142" t="n">
+      <c r="E142" t="n">
         <v>-13.29</v>
       </c>
     </row>
     <row r="143">
-      <c r="A143" t="n">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>148 SW2R</t>
+        </is>
+      </c>
+      <c r="B143" t="n">
         <v>-21.14</v>
       </c>
-      <c r="B143" t="n">
+      <c r="C143" t="n">
         <v>2.98</v>
       </c>
-      <c r="C143" t="n">
+      <c r="D143" t="n">
         <v>-9.17</v>
       </c>
-      <c r="D143" t="n">
+      <c r="E143" t="n">
         <v>-10.01</v>
       </c>
     </row>
     <row r="144">
-      <c r="A144" t="n">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>149 SW3H</t>
+        </is>
+      </c>
+      <c r="B144" t="n">
         <v>-17.94</v>
       </c>
-      <c r="B144" t="n">
+      <c r="C144" t="n">
         <v>6.97</v>
       </c>
-      <c r="C144" t="n">
+      <c r="D144" t="n">
         <v>-8.5</v>
       </c>
-      <c r="D144" t="n">
+      <c r="E144" t="n">
         <v>-11.51</v>
       </c>
     </row>
     <row r="145">
-      <c r="A145" t="n">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>150 SW4F</t>
+        </is>
+      </c>
+      <c r="B145" t="n">
         <v>-20.73</v>
       </c>
-      <c r="B145" t="n">
+      <c r="C145" t="n">
         <v>8.68</v>
       </c>
-      <c r="C145" t="n">
+      <c r="D145" t="n">
         <v>-12.19</v>
       </c>
-      <c r="D145" t="n">
+      <c r="E145" t="n">
         <v>-11.35</v>
       </c>
     </row>
     <row r="146">
-      <c r="A146" t="n">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>151 SW5Tt</t>
+        </is>
+      </c>
+      <c r="B146" t="n">
         <v>-21.01</v>
       </c>
-      <c r="B146" t="n">
+      <c r="C146" t="n">
         <v>8.359999999999999</v>
       </c>
-      <c r="C146" t="n">
+      <c r="D146" t="n">
         <v>-12.49</v>
       </c>
-      <c r="D146" t="n">
+      <c r="E146" t="n">
         <v>-12.84</v>
       </c>
     </row>
     <row r="147">
-      <c r="A147" t="n">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>Hb 123</t>
+        </is>
+      </c>
+      <c r="B147" t="n">
         <v>-12.45</v>
       </c>
-      <c r="B147" t="n">
+      <c r="C147" t="n">
         <v>7.14</v>
       </c>
-      <c r="C147" t="n">
+      <c r="D147" t="n">
         <v>-6.73</v>
       </c>
-      <c r="D147" t="n">
+      <c r="E147" t="n">
         <v>-6.72</v>
       </c>
     </row>
     <row r="148">
-      <c r="A148" t="n">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>Hb 124</t>
+        </is>
+      </c>
+      <c r="B148" t="n">
         <v>-19.36</v>
       </c>
-      <c r="B148" t="n">
+      <c r="C148" t="n">
         <v>5.76</v>
       </c>
-      <c r="C148" t="n">
+      <c r="D148" t="n">
         <v>-12.73</v>
       </c>
-      <c r="D148" t="n">
+      <c r="E148" t="n">
         <v>-9.06</v>
       </c>
     </row>
     <row r="149">
-      <c r="A149" t="n">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>Hb 125</t>
+        </is>
+      </c>
+      <c r="B149" t="n">
         <v>-24.32</v>
       </c>
-      <c r="B149" t="n">
+      <c r="C149" t="n">
         <v>9.48</v>
       </c>
-      <c r="C149" t="n">
+      <c r="D149" t="n">
         <v>-18.06</v>
       </c>
-      <c r="D149" t="n">
+      <c r="E149" t="n">
         <v>-10.18</v>
       </c>
     </row>
     <row r="150">
-      <c r="A150" t="n">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>S 56</t>
+        </is>
+      </c>
+      <c r="B150" t="n">
         <v>-20.94</v>
       </c>
-      <c r="B150" t="n">
+      <c r="C150" t="n">
         <v>10.44</v>
       </c>
-      <c r="C150" t="n">
+      <c r="D150" t="n">
         <v>-13.38</v>
       </c>
-      <c r="D150" t="n">
+      <c r="E150" t="n">
         <v>-8.550000000000001</v>
       </c>
     </row>
     <row r="151">
-      <c r="A151" t="n">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>S 57</t>
+        </is>
+      </c>
+      <c r="B151" t="n">
         <v>-23.52</v>
       </c>
-      <c r="B151" t="n">
+      <c r="C151" t="n">
         <v>7.96</v>
       </c>
-      <c r="C151" t="n">
+      <c r="D151" t="n">
         <v>-14.08</v>
       </c>
-      <c r="D151" t="n">
+      <c r="E151" t="n">
         <v>-12.52</v>
       </c>
     </row>
     <row r="152">
-      <c r="A152" t="n">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>S 58</t>
+        </is>
+      </c>
+      <c r="B152" t="n">
         <v>-12.49</v>
       </c>
-      <c r="B152" t="n">
+      <c r="C152" t="n">
         <v>10.23</v>
       </c>
-      <c r="C152" t="n">
+      <c r="D152" t="n">
         <v>-7.25</v>
       </c>
-      <c r="D152" t="n">
+      <c r="E152" t="n">
         <v>-9.300000000000001</v>
       </c>
     </row>
     <row r="153">
-      <c r="A153" t="n">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>Hb 131</t>
+        </is>
+      </c>
+      <c r="B153" t="n">
         <v>-24.11</v>
       </c>
-      <c r="B153" t="n">
+      <c r="C153" t="n">
         <v>7.65</v>
       </c>
-      <c r="C153" t="n">
+      <c r="D153" t="n">
         <v>-16.44</v>
       </c>
-      <c r="D153" t="n">
+      <c r="E153" t="n">
         <v>-10.54</v>
       </c>
     </row>
     <row r="154">
-      <c r="A154" t="n">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>Hb 133</t>
+        </is>
+      </c>
+      <c r="B154" t="n">
         <v>-21.26</v>
       </c>
-      <c r="B154" t="n">
+      <c r="C154" t="n">
         <v>8.42</v>
       </c>
-      <c r="C154" t="n">
+      <c r="D154" t="n">
         <v>-12.29</v>
       </c>
-      <c r="D154" t="n">
+      <c r="E154" t="n">
         <v>-7.81</v>
       </c>
     </row>
     <row r="155">
-      <c r="A155" t="n">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>Hb 134</t>
+        </is>
+      </c>
+      <c r="B155" t="n">
         <v>-21.29</v>
       </c>
-      <c r="B155" t="n">
+      <c r="C155" t="n">
         <v>7.86</v>
       </c>
-      <c r="C155" t="n">
+      <c r="D155" t="n">
         <v>-12.45</v>
       </c>
-      <c r="D155" t="n">
+      <c r="E155" t="n">
         <v>-8.83</v>
       </c>
     </row>
     <row r="156">
-      <c r="A156" t="n">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>S 46</t>
+        </is>
+      </c>
+      <c r="B156" t="n">
         <v>-20.6</v>
       </c>
-      <c r="B156" t="n">
+      <c r="C156" t="n">
         <v>10.41</v>
       </c>
-      <c r="C156" t="n">
+      <c r="D156" t="n">
         <v>-12.85</v>
       </c>
-      <c r="D156" t="n">
+      <c r="E156" t="n">
         <v>-6.91</v>
       </c>
     </row>
     <row r="157">
-      <c r="A157" t="n">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>S 47</t>
+        </is>
+      </c>
+      <c r="B157" t="n">
         <v>-21.47</v>
       </c>
-      <c r="B157" t="n">
+      <c r="C157" t="n">
         <v>11.88</v>
       </c>
-      <c r="C157" t="n">
+      <c r="D157" t="n">
         <v>-13.32</v>
       </c>
-      <c r="D157" t="n">
+      <c r="E157" t="n">
         <v>-7.43</v>
       </c>
     </row>
     <row r="158">
-      <c r="A158" t="n">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>S 48</t>
+        </is>
+      </c>
+      <c r="B158" t="n">
         <v>-23.33</v>
       </c>
-      <c r="B158" t="n">
+      <c r="C158" t="n">
         <v>7.6</v>
       </c>
-      <c r="C158" t="n">
+      <c r="D158" t="n">
         <v>-15.09</v>
       </c>
-      <c r="D158" t="n">
+      <c r="E158" t="n">
         <v>-8.19</v>
       </c>
     </row>
     <row r="159">
-      <c r="A159" t="n">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>S 49</t>
+        </is>
+      </c>
+      <c r="B159" t="n">
         <v>-20.43</v>
       </c>
-      <c r="B159" t="n">
+      <c r="C159" t="n">
         <v>10.36</v>
       </c>
-      <c r="C159" t="n">
+      <c r="D159" t="n">
         <v>-11.44</v>
       </c>
-      <c r="D159" t="n">
+      <c r="E159" t="n">
         <v>-8.539999999999999</v>
       </c>
     </row>
     <row r="160">
-      <c r="A160" t="n">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>S 50</t>
+        </is>
+      </c>
+      <c r="B160" t="n">
         <v>-23.6</v>
       </c>
-      <c r="B160" t="n">
+      <c r="C160" t="n">
         <v>12.62</v>
       </c>
-      <c r="C160" t="n">
+      <c r="D160" t="n">
         <v>-14.85</v>
       </c>
-      <c r="D160" t="n">
+      <c r="E160" t="n">
         <v>-9.880000000000001</v>
       </c>
     </row>
     <row r="161">
-      <c r="A161" t="n">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>104 SE2H</t>
+        </is>
+      </c>
+      <c r="B161" t="n">
         <v>-23.13</v>
       </c>
-      <c r="B161" t="n">
+      <c r="C161" t="n">
         <v>7.64</v>
       </c>
-      <c r="C161" t="n">
+      <c r="D161" t="n">
         <v>-12.89</v>
       </c>
-      <c r="D161" t="n">
+      <c r="E161" t="n">
         <v>-9.57</v>
       </c>
     </row>
     <row r="162">
-      <c r="A162" t="n">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>105 SE3U</t>
+        </is>
+      </c>
+      <c r="B162" t="n">
         <v>-20.35</v>
       </c>
-      <c r="B162" t="n">
+      <c r="C162" t="n">
         <v>9.84</v>
       </c>
-      <c r="C162" t="n">
+      <c r="D162" t="n">
         <v>-9.710000000000001</v>
       </c>
-      <c r="D162" t="n">
+      <c r="E162" t="n">
         <v>-7.82</v>
       </c>
     </row>
     <row r="163">
-      <c r="A163" t="n">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>152 SE1H</t>
+        </is>
+      </c>
+      <c r="B163" t="n">
         <v>-16.84</v>
       </c>
-      <c r="B163" t="n">
+      <c r="C163" t="n">
         <v>15.48</v>
       </c>
-      <c r="C163" t="n">
+      <c r="D163" t="n">
         <v>-10.45</v>
       </c>
-      <c r="D163" t="n">
+      <c r="E163" t="n">
         <v>-6.71</v>
       </c>
     </row>
     <row r="164">
-      <c r="A164" t="n">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>153 SE2H</t>
+        </is>
+      </c>
+      <c r="B164" t="n">
         <v>-12.71</v>
       </c>
-      <c r="B164" t="n">
+      <c r="C164" t="n">
         <v>12.92</v>
       </c>
-      <c r="C164" t="n">
+      <c r="D164" t="n">
         <v>-6.56</v>
       </c>
-      <c r="D164" t="n">
+      <c r="E164" t="n">
         <v>-8.550000000000001</v>
       </c>
     </row>
     <row r="165">
-      <c r="A165" t="n">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>154 SE3H</t>
+        </is>
+      </c>
+      <c r="B165" t="n">
         <v>-21.54</v>
       </c>
-      <c r="B165" t="n">
+      <c r="C165" t="n">
         <v>8.56</v>
       </c>
-      <c r="C165" t="n">
+      <c r="D165" t="n">
         <v>-13.23</v>
       </c>
-      <c r="D165" t="n">
+      <c r="E165" t="n">
         <v>-7.69</v>
       </c>
     </row>
     <row r="166">
-      <c r="A166" t="n">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>155 SE4H</t>
+        </is>
+      </c>
+      <c r="B166" t="n">
         <v>-19.63</v>
       </c>
-      <c r="B166" t="n">
+      <c r="C166" t="n">
         <v>10.43</v>
       </c>
-      <c r="C166" t="n">
+      <c r="D166" t="n">
         <v>-13.77</v>
       </c>
-      <c r="D166" t="n">
+      <c r="E166" t="n">
         <v>-11.72</v>
       </c>
     </row>
     <row r="167">
-      <c r="A167" t="n">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>156 SE5H</t>
+        </is>
+      </c>
+      <c r="B167" t="n">
         <v>-23.47</v>
       </c>
-      <c r="B167" t="n">
+      <c r="C167" t="n">
         <v>4.93</v>
       </c>
-      <c r="C167" t="n">
+      <c r="D167" t="n">
         <v>-13.21</v>
       </c>
-      <c r="D167" t="n">
+      <c r="E167" t="n">
         <v>-9.630000000000001</v>
       </c>
     </row>
     <row r="168">
-      <c r="A168" t="n">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>Hb 178</t>
+        </is>
+      </c>
+      <c r="B168" t="n">
         <v>-17.5</v>
       </c>
-      <c r="B168" t="n">
+      <c r="C168" t="n">
         <v>14.15</v>
       </c>
-      <c r="C168" t="n">
+      <c r="D168" t="n">
         <v>-11.68</v>
       </c>
-      <c r="D168" t="n">
+      <c r="E168" t="n">
         <v>-8.68</v>
       </c>
     </row>
     <row r="169">
-      <c r="A169" t="n">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>Hb 179</t>
+        </is>
+      </c>
+      <c r="B169" t="n">
         <v>-17.1</v>
       </c>
-      <c r="B169" t="n">
+      <c r="C169" t="n">
         <v>12.74</v>
       </c>
-      <c r="C169" t="n">
+      <c r="D169" t="n">
         <v>-10.43</v>
       </c>
-      <c r="D169" t="n">
+      <c r="E169" t="n">
         <v>-7.21</v>
       </c>
     </row>
     <row r="170">
-      <c r="A170" t="n">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>Hb 180</t>
+        </is>
+      </c>
+      <c r="B170" t="n">
         <v>-15.83</v>
       </c>
-      <c r="B170" t="n">
+      <c r="C170" t="n">
         <v>15.12</v>
       </c>
-      <c r="C170" t="n">
+      <c r="D170" t="n">
         <v>-11.06</v>
       </c>
-      <c r="D170" t="n">
+      <c r="E170" t="n">
         <v>-5.07</v>
       </c>
     </row>
     <row r="171">
-      <c r="A171" t="n">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>Hb 182</t>
+        </is>
+      </c>
+      <c r="B171" t="n">
         <v>-15.5</v>
       </c>
-      <c r="B171" t="n">
+      <c r="C171" t="n">
         <v>16.43</v>
       </c>
-      <c r="C171" t="n">
+      <c r="D171" t="n">
         <v>-9.470000000000001</v>
       </c>
-      <c r="D171" t="n">
+      <c r="E171" t="n">
         <v>-4.1</v>
       </c>
     </row>
     <row r="172">
-      <c r="A172" t="n">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>109 TL2St</t>
+        </is>
+      </c>
+      <c r="B172" t="n">
         <v>-17.11</v>
       </c>
-      <c r="B172" t="n">
+      <c r="C172" t="n">
         <v>13.53</v>
       </c>
-      <c r="C172" t="n">
+      <c r="D172" t="n">
         <v>-6.57</v>
       </c>
-      <c r="D172" t="n">
+      <c r="E172" t="n">
         <v>-7.26</v>
       </c>
     </row>
     <row r="173">
-      <c r="A173" t="n">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>110 TL3St</t>
+        </is>
+      </c>
+      <c r="B173" t="n">
         <v>-16.25</v>
       </c>
-      <c r="B173" t="n">
+      <c r="C173" t="n">
         <v>13.86</v>
       </c>
-      <c r="C173" t="n">
+      <c r="D173" t="n">
         <v>-4.94</v>
       </c>
-      <c r="D173" t="n">
+      <c r="E173" t="n">
         <v>-5.05</v>
       </c>
     </row>
     <row r="174">
-      <c r="A174" t="n">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>S 91</t>
+        </is>
+      </c>
+      <c r="B174" t="n">
         <v>-20.29</v>
       </c>
-      <c r="B174" t="n">
+      <c r="C174" t="n">
         <v>10.99</v>
       </c>
-      <c r="C174" t="n">
+      <c r="D174" t="n">
         <v>-10</v>
       </c>
-      <c r="D174" t="n">
+      <c r="E174" t="n">
         <v>-6.16</v>
       </c>
     </row>
     <row r="175">
-      <c r="A175" t="n">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>S 92</t>
+        </is>
+      </c>
+      <c r="B175" t="n">
         <v>-20.48</v>
       </c>
-      <c r="B175" t="n">
+      <c r="C175" t="n">
         <v>10.84</v>
       </c>
-      <c r="C175" t="n">
+      <c r="D175" t="n">
         <v>-8.99</v>
       </c>
-      <c r="D175" t="n">
+      <c r="E175" t="n">
         <v>-8.380000000000001</v>
       </c>
     </row>
     <row r="176">
-      <c r="A176" t="n">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>S 93</t>
+        </is>
+      </c>
+      <c r="B176" t="n">
         <v>-19.01</v>
       </c>
-      <c r="B176" t="n">
+      <c r="C176" t="n">
         <v>9.66</v>
       </c>
-      <c r="C176" t="n">
+      <c r="D176" t="n">
         <v>-8.42</v>
       </c>
-      <c r="D176" t="n">
+      <c r="E176" t="n">
         <v>-7.31</v>
       </c>
     </row>
     <row r="177">
-      <c r="A177" t="n">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>S 94</t>
+        </is>
+      </c>
+      <c r="B177" t="n">
         <v>-19.2</v>
       </c>
-      <c r="B177" t="n">
+      <c r="C177" t="n">
         <v>8.08</v>
       </c>
-      <c r="C177" t="n">
+      <c r="D177" t="n">
         <v>-8.84</v>
       </c>
-      <c r="D177" t="n">
+      <c r="E177" t="n">
         <v>-10.88</v>
       </c>
     </row>
     <row r="178">
-      <c r="A178" t="n">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>S 66</t>
+        </is>
+      </c>
+      <c r="B178" t="n">
         <v>-18.26</v>
       </c>
-      <c r="B178" t="n">
+      <c r="C178" t="n">
         <v>9.1</v>
       </c>
-      <c r="C178" t="n">
+      <c r="D178" t="n">
         <v>-10.98</v>
       </c>
-      <c r="D178" t="n">
+      <c r="E178" t="n">
         <v>-11.57</v>
       </c>
     </row>

</xml_diff>